<commit_message>
Cucumber Lessons Repeating with Jenkins Examples
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="17">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>04.04.23</t>
+  </si>
+  <si>
+    <t>07.04.23</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="K78" sqref="K78"/>
@@ -1748,6 +1751,20 @@
         <v>15</v>
       </c>
     </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>10</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" t="s">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cucumber Lessons Repeating with Jenkins Examples after merging
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="17">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -424,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="K78" sqref="K78"/>
@@ -1779,6 +1779,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>10</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" t="s">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
country functionality set wrong on purpose to get the cucumber reports 2
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resource/ScenarioStatus.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="17">
   <si>
     <t>Login with valid username and password</t>
   </si>
@@ -424,7 +424,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
       <selection activeCell="K78" sqref="K78"/>
@@ -1793,6 +1793,20 @@
         <v>16</v>
       </c>
     </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>10</v>
+      </c>
+      <c r="B98" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>